<commit_message>
Bookkeeping on fractionation data
</commit_message>
<xml_diff>
--- a/data/fractionation/221109 Batch 129 Water Year Summary.xlsx
+++ b/data/fractionation/221109 Batch 129 Water Year Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Banfield\WaterYear\SIP\data\fractionation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF138DDC-ADDE-41E6-8622-70F3EBAEA2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABC716-F25B-4091-865D-6FB528CC181C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="622" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="22" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="245">
   <si>
     <t>calculated density p(20)</t>
   </si>
@@ -787,9 +787,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -884,12 +881,6 @@
   </si>
   <si>
     <t>3957-conc</t>
-  </si>
-  <si>
-    <t>3193-density</t>
-  </si>
-  <si>
-    <t>3193-conc</t>
   </si>
   <si>
     <t>3198-density</t>
@@ -1055,7 +1046,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1095,12 +1086,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1262,7 +1247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1494,10 +1479,6 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="8" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5316,7 +5297,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AD$4:$AD$25</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -5509,7 +5490,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AG$4:$AG$25</c:f>
+              <c:f>Summary!$AD$4:$AD$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -5702,7 +5683,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AJ$4:$AJ$25</c:f>
+              <c:f>Summary!$AG$4:$AG$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -5898,7 +5879,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AM$4:$AM$25</c:f>
+              <c:f>Summary!$AJ$4:$AJ$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -6094,7 +6075,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AP$4:$AP$25</c:f>
+              <c:f>Summary!$AM$4:$AM$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -6290,7 +6271,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AS$4:$AS$25</c:f>
+              <c:f>Summary!$AP$4:$AP$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -6486,7 +6467,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AV$4:$AV$25</c:f>
+              <c:f>Summary!$AS$4:$AS$25</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="22"/>
@@ -7203,132 +7184,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AD$5:$AD$23</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1.7758225110000012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7681731910000025</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7616166310000008</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7563440640000021</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7497875040000022</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7619990970000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.737958377</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7467004570000029</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.7326858100000013</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7195726899999997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.714300123000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.7088363230000017</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.7011870029999994</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6946304430000012</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6891666430000019</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6828013160000026</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6762447560000009</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.6620388760000022</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.5997515560000011</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Summary!#REF!</c:f>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AE$5:$AE$23</c:f>
+              <c:f>Summary!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-2.2744805687566292E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.1746969907379024E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.069589655491865E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.3911836393426142E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.17726908426687879</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.68477902703551463</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1653297508468299</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0272573685676323</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.1297521523685372</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12.790632613549747</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.6880382036748482</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.4817869109138084</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.4925442748630395</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.73640113105829552</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.40619333424236964</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.21686418843300589</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.13107286315389047</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.1273326074937754</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.16686307307424886</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7378,7 +7244,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AG$5:$AG$23</c:f>
+              <c:f>Summary!$AD$5:$AD$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7444,7 +7310,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AH$5:$AH$23</c:f>
+              <c:f>Summary!$AE$5:$AE$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7553,7 +7419,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AJ$5:$AJ$23</c:f>
+              <c:f>Summary!$AG$5:$AG$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7619,7 +7485,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AK$5:$AK$23</c:f>
+              <c:f>Summary!$AH$5:$AH$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7731,7 +7597,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AM$5:$AM$23</c:f>
+              <c:f>Summary!$AJ$5:$AJ$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7797,7 +7663,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AN$5:$AN$23</c:f>
+              <c:f>Summary!$AK$5:$AK$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7909,7 +7775,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AP$5:$AP$23</c:f>
+              <c:f>Summary!$AM$5:$AM$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -7975,7 +7841,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AQ$5:$AQ$23</c:f>
+              <c:f>Summary!$AN$5:$AN$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -8087,7 +7953,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AS$5:$AS$23</c:f>
+              <c:f>Summary!$AP$5:$AP$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -8153,7 +8019,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AT$5:$AT$23</c:f>
+              <c:f>Summary!$AQ$5:$AQ$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -8265,7 +8131,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Summary!$AV$5:$AV$23</c:f>
+              <c:f>Summary!$AS$5:$AS$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -8331,7 +8197,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Summary!$AW$5:$AW$23</c:f>
+              <c:f>Summary!$AT$5:$AT$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="19"/>
@@ -12139,10 +12005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E138FBF1-D534-4F7E-950C-764D2E6B8C19}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -12185,16 +12051,16 @@
         <v>196</v>
       </c>
       <c r="F4" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="G4" s="27" t="s">
         <v>205</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>206</v>
       </c>
       <c r="H4" s="27" t="s">
         <v>197</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J4" s="27" t="s">
         <v>194</v>
@@ -12472,12 +12338,12 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="66">
-        <f>'Tube Loading'!F38</f>
-        <v>3193</v>
+        <f>'Tube Loading'!F39</f>
+        <v>3198</v>
       </c>
       <c r="B14" s="66" t="str">
-        <f>'Tube Loading'!A38</f>
-        <v>Tube J</v>
+        <f>'Tube Loading'!A39</f>
+        <v>Tube K</v>
       </c>
       <c r="C14" s="66" t="s">
         <v>198</v>
@@ -12489,25 +12355,25 @@
         <v>130</v>
       </c>
       <c r="G14" s="66">
-        <f>'Tube Loading'!K38</f>
+        <f>'Tube Loading'!K39</f>
         <v>4000</v>
       </c>
       <c r="H14" s="50">
         <f>Summary!AE26</f>
-        <v>40.552989377242596</v>
-      </c>
-      <c r="I14" s="50">
+        <v>53.948770902690413</v>
+      </c>
+      <c r="I14" s="68">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="66">
-        <f>'Tube Loading'!F39</f>
-        <v>3198</v>
+        <f>'Tube Loading'!F40</f>
+        <v>1425</v>
       </c>
       <c r="B15" s="66" t="str">
-        <f>'Tube Loading'!A39</f>
-        <v>Tube K</v>
+        <f>'Tube Loading'!A40</f>
+        <v>Tube L</v>
       </c>
       <c r="C15" s="66" t="s">
         <v>198</v>
@@ -12519,55 +12385,55 @@
         <v>130</v>
       </c>
       <c r="G15" s="66">
-        <f>'Tube Loading'!K39</f>
+        <f>'Tube Loading'!K40</f>
         <v>4000</v>
       </c>
       <c r="H15" s="50">
         <f>Summary!AH26</f>
-        <v>53.948770902690413</v>
-      </c>
-      <c r="I15" s="68">
+        <v>58.371507777243245</v>
+      </c>
+      <c r="I15" s="50">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="66">
-        <f>'Tube Loading'!F40</f>
-        <v>1425</v>
+        <f>'Tube Loading'!F41</f>
+        <v>3967</v>
       </c>
       <c r="B16" s="66" t="str">
-        <f>'Tube Loading'!A40</f>
-        <v>Tube L</v>
+        <f>'Tube Loading'!A41</f>
+        <v>Tube M</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D16" s="67">
         <v>44874</v>
       </c>
       <c r="E16">
-        <v>130</v>
+        <v>133.5</v>
       </c>
       <c r="G16" s="66">
-        <f>'Tube Loading'!K40</f>
+        <f>'Tube Loading'!K41</f>
         <v>4000</v>
       </c>
       <c r="H16" s="50">
         <f>Summary!AK26</f>
-        <v>58.371507777243245</v>
-      </c>
-      <c r="I16" s="50">
+        <v>75.763760038666732</v>
+      </c>
+      <c r="I16" s="68">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="66">
-        <f>'Tube Loading'!F41</f>
-        <v>3967</v>
+        <f>'Tube Loading'!F42</f>
+        <v>3644</v>
       </c>
       <c r="B17" s="66" t="str">
-        <f>'Tube Loading'!A41</f>
-        <v>Tube M</v>
+        <f>'Tube Loading'!A42</f>
+        <v>Tube N</v>
       </c>
       <c r="C17" s="66" t="s">
         <v>199</v>
@@ -12579,25 +12445,25 @@
         <v>133.5</v>
       </c>
       <c r="G17" s="66">
-        <f>'Tube Loading'!K41</f>
+        <f>'Tube Loading'!K42</f>
         <v>4000</v>
       </c>
       <c r="H17" s="50">
         <f>Summary!AN26</f>
-        <v>75.763760038666732</v>
-      </c>
-      <c r="I17" s="68">
+        <v>78.869964770790631</v>
+      </c>
+      <c r="I17" s="50">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="66">
-        <f>'Tube Loading'!F42</f>
-        <v>3644</v>
+        <f>'Tube Loading'!F43</f>
+        <v>1441</v>
       </c>
       <c r="B18" s="66" t="str">
-        <f>'Tube Loading'!A42</f>
-        <v>Tube N</v>
+        <f>'Tube Loading'!A43</f>
+        <v>Tube O</v>
       </c>
       <c r="C18" s="66" t="s">
         <v>199</v>
@@ -12609,25 +12475,25 @@
         <v>133.5</v>
       </c>
       <c r="G18" s="66">
-        <f>'Tube Loading'!K42</f>
+        <f>'Tube Loading'!K43</f>
         <v>4000</v>
       </c>
       <c r="H18" s="50">
         <f>Summary!AQ26</f>
-        <v>78.869964770790631</v>
-      </c>
-      <c r="I18" s="50">
+        <v>74.347533564064079</v>
+      </c>
+      <c r="I18" s="68">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="66">
-        <f>'Tube Loading'!F43</f>
-        <v>1441</v>
+        <f>'Tube Loading'!F44</f>
+        <v>1789</v>
       </c>
       <c r="B19" s="66" t="str">
-        <f>'Tube Loading'!A43</f>
-        <v>Tube O</v>
+        <f>'Tube Loading'!A44</f>
+        <v>Tube P</v>
       </c>
       <c r="C19" s="66" t="s">
         <v>199</v>
@@ -12639,55 +12505,25 @@
         <v>133.5</v>
       </c>
       <c r="G19" s="66">
-        <f>'Tube Loading'!K43</f>
+        <f>'Tube Loading'!K44</f>
         <v>4000</v>
       </c>
       <c r="H19" s="50">
         <f>Summary!AT26</f>
-        <v>74.347533564064079</v>
-      </c>
-      <c r="I19" s="68">
+        <v>46.076539466850186</v>
+      </c>
+      <c r="I19" s="50">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="66">
-        <f>'Tube Loading'!F44</f>
-        <v>1789</v>
-      </c>
-      <c r="B20" s="66" t="str">
-        <f>'Tube Loading'!A44</f>
-        <v>Tube P</v>
-      </c>
-      <c r="C20" s="66" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="67">
-        <v>44874</v>
-      </c>
-      <c r="E20">
-        <v>133.5</v>
-      </c>
-      <c r="G20" s="66">
-        <f>'Tube Loading'!K44</f>
-        <v>4000</v>
-      </c>
-      <c r="H20" s="50">
-        <f>Summary!AW26</f>
-        <v>46.076539466850186</v>
-      </c>
-      <c r="I20" s="50">
-        <v>37</v>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -21297,10 +21133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA4E3B1-5772-4D1F-AF5A-033072A123CA}">
-  <dimension ref="A1:AW85"/>
+  <dimension ref="A1:AT85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN34" sqref="AN34"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.5"/>
@@ -21315,7 +21151,7 @@
     <col min="12" max="16384" width="10.81640625" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:46">
       <c r="A1" s="62" t="s">
         <v>183</v>
       </c>
@@ -21323,233 +21159,219 @@
         <v>1455</v>
       </c>
       <c r="C1" s="56" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="56" t="s">
         <v>216</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>217</v>
       </c>
       <c r="E1" s="56">
         <v>3964</v>
       </c>
       <c r="F1" s="56" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" s="56" t="s">
         <v>218</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>219</v>
       </c>
       <c r="H1" s="56">
         <v>2034</v>
       </c>
       <c r="I1" s="56" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="56" t="s">
         <v>220</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>221</v>
       </c>
       <c r="K1" s="56">
         <v>3200</v>
       </c>
       <c r="L1" s="56" t="s">
+        <v>221</v>
+      </c>
+      <c r="M1" s="56" t="s">
         <v>222</v>
-      </c>
-      <c r="M1" s="56" t="s">
-        <v>223</v>
       </c>
       <c r="N1" s="56">
         <v>2041</v>
       </c>
       <c r="O1" s="56" t="s">
+        <v>223</v>
+      </c>
+      <c r="P1" s="56" t="s">
         <v>224</v>
-      </c>
-      <c r="P1" s="56" t="s">
-        <v>225</v>
       </c>
       <c r="Q1" s="56">
         <v>4004</v>
       </c>
       <c r="R1" s="56" t="s">
+        <v>225</v>
+      </c>
+      <c r="S1" s="56" t="s">
         <v>226</v>
-      </c>
-      <c r="S1" s="56" t="s">
-        <v>227</v>
       </c>
       <c r="T1" s="56">
         <v>3969</v>
       </c>
       <c r="U1" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="V1" s="56" t="s">
         <v>228</v>
-      </c>
-      <c r="V1" s="56" t="s">
-        <v>229</v>
       </c>
       <c r="W1" s="56">
         <v>1792</v>
       </c>
       <c r="X1" s="56" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y1" s="56" t="s">
         <v>230</v>
-      </c>
-      <c r="Y1" s="56" t="s">
-        <v>231</v>
       </c>
       <c r="Z1" s="56">
         <v>3957</v>
       </c>
       <c r="AA1" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="AB1" s="56" t="s">
         <v>232</v>
       </c>
-      <c r="AB1" s="56" t="s">
+      <c r="AC1" s="56">
+        <v>3198</v>
+      </c>
+      <c r="AD1" s="56" t="s">
         <v>233</v>
       </c>
-      <c r="AC1" s="56">
-        <v>3193</v>
-      </c>
-      <c r="AD1" s="56" t="s">
+      <c r="AE1" s="56" t="s">
         <v>234</v>
       </c>
-      <c r="AE1" s="56" t="s">
+      <c r="AF1" s="56">
+        <v>1425</v>
+      </c>
+      <c r="AG1" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="AF1" s="56">
-        <v>3198</v>
-      </c>
-      <c r="AG1" s="56" t="s">
+      <c r="AH1" s="56" t="s">
         <v>236</v>
       </c>
-      <c r="AH1" s="56" t="s">
+      <c r="AI1" s="56">
+        <v>3967</v>
+      </c>
+      <c r="AJ1" s="56" t="s">
         <v>237</v>
       </c>
-      <c r="AI1" s="56">
-        <v>1425</v>
-      </c>
-      <c r="AJ1" s="56" t="s">
+      <c r="AK1" s="56" t="s">
         <v>238</v>
       </c>
-      <c r="AK1" s="56" t="s">
+      <c r="AL1" s="56">
+        <v>3644</v>
+      </c>
+      <c r="AM1" s="56" t="s">
         <v>239</v>
       </c>
-      <c r="AL1" s="56">
-        <v>3967</v>
-      </c>
-      <c r="AM1" s="56" t="s">
+      <c r="AN1" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="AN1" s="56" t="s">
+      <c r="AO1" s="56">
+        <v>1441</v>
+      </c>
+      <c r="AP1" s="56" t="s">
         <v>241</v>
       </c>
-      <c r="AO1" s="56">
-        <v>3644</v>
-      </c>
-      <c r="AP1" s="56" t="s">
+      <c r="AQ1" s="56" t="s">
         <v>242</v>
       </c>
-      <c r="AQ1" s="56" t="s">
+      <c r="AR1" s="56">
+        <v>1789</v>
+      </c>
+      <c r="AS1" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="AR1" s="56">
-        <v>1441</v>
-      </c>
-      <c r="AS1" s="56" t="s">
+      <c r="AT1" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="AT1" s="56" t="s">
-        <v>245</v>
-      </c>
-      <c r="AU1" s="56">
-        <v>1789</v>
-      </c>
-      <c r="AV1" s="56" t="s">
-        <v>246</v>
-      </c>
-      <c r="AW1" s="56" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="2" spans="1:49">
+    </row>
+    <row r="2" spans="1:46">
       <c r="A2" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="113" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="115" t="s">
+      <c r="C2" s="114"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="113" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="116"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="115" t="s">
+      <c r="F2" s="114"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="113" t="s">
         <v>168</v>
       </c>
-      <c r="I2" s="116"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="115" t="s">
+      <c r="I2" s="114"/>
+      <c r="J2" s="115"/>
+      <c r="K2" s="113" t="s">
         <v>169</v>
       </c>
-      <c r="L2" s="116"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="112" t="s">
+      <c r="L2" s="114"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="110" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="113"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="112" t="s">
+      <c r="O2" s="111"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="110" t="s">
         <v>172</v>
       </c>
-      <c r="R2" s="113"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="112" t="s">
+      <c r="R2" s="111"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="110" t="s">
         <v>173</v>
       </c>
-      <c r="U2" s="113"/>
-      <c r="V2" s="114"/>
-      <c r="W2" s="112" t="s">
+      <c r="U2" s="111"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="110" t="s">
         <v>174</v>
       </c>
-      <c r="X2" s="113"/>
-      <c r="Y2" s="114"/>
-      <c r="Z2" s="112" t="s">
+      <c r="X2" s="111"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="110" t="s">
         <v>200</v>
       </c>
-      <c r="AA2" s="113"/>
-      <c r="AB2" s="114"/>
-      <c r="AC2" s="112" t="s">
+      <c r="AA2" s="111"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="110" t="s">
         <v>201</v>
       </c>
-      <c r="AD2" s="113"/>
-      <c r="AE2" s="114"/>
-      <c r="AF2" s="112" t="s">
+      <c r="AD2" s="111"/>
+      <c r="AE2" s="112"/>
+      <c r="AF2" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="111"/>
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="110" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ2" s="111"/>
+      <c r="AK2" s="112"/>
+      <c r="AL2" s="110" t="s">
+        <v>23</v>
+      </c>
+      <c r="AM2" s="111"/>
+      <c r="AN2" s="112"/>
+      <c r="AO2" s="110" t="s">
         <v>202</v>
       </c>
-      <c r="AG2" s="113"/>
-      <c r="AH2" s="114"/>
-      <c r="AI2" s="112" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ2" s="113"/>
-      <c r="AK2" s="114"/>
-      <c r="AL2" s="112" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM2" s="113"/>
-      <c r="AN2" s="114"/>
-      <c r="AO2" s="112" t="s">
-        <v>23</v>
-      </c>
-      <c r="AP2" s="113"/>
-      <c r="AQ2" s="114"/>
-      <c r="AR2" s="112" t="s">
+      <c r="AP2" s="111"/>
+      <c r="AQ2" s="112"/>
+      <c r="AR2" s="110" t="s">
         <v>203</v>
       </c>
-      <c r="AS2" s="113"/>
-      <c r="AT2" s="114"/>
-      <c r="AU2" s="112" t="s">
-        <v>204</v>
-      </c>
-      <c r="AV2" s="113"/>
-      <c r="AW2" s="114"/>
-    </row>
-    <row r="3" spans="1:49">
+      <c r="AS2" s="111"/>
+      <c r="AT2" s="112"/>
+    </row>
+    <row r="3" spans="1:46">
       <c r="A3" s="62" t="s">
         <v>165</v>
       </c>
@@ -21688,17 +21510,8 @@
       <c r="AT3" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="AU3" s="84" t="s">
-        <v>185</v>
-      </c>
-      <c r="AV3" s="85" t="s">
-        <v>186</v>
-      </c>
-      <c r="AW3" s="86" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49">
+    </row>
+    <row r="4" spans="1:46">
       <c r="A4" s="56">
         <v>1</v>
       </c>
@@ -21802,84 +21615,73 @@
         <v>9.25687035360339E-3</v>
       </c>
       <c r="AC4" s="69" t="str">
-        <f>'Tube J'!G2</f>
-        <v>G3</v>
-      </c>
-      <c r="AD4" s="70">
-        <f>'Tube J'!F2</f>
-        <v>1.720091751</v>
-      </c>
-      <c r="AE4" s="71">
-        <v>-1.2697668712026345E-2</v>
-      </c>
-      <c r="AF4" s="69" t="str">
         <f>'Tube K'!G2</f>
         <v>D6</v>
       </c>
-      <c r="AG4" s="70">
+      <c r="AD4" s="70">
         <f>'Tube K'!F2</f>
         <v>1.7179608690000006</v>
       </c>
-      <c r="AH4" s="71">
+      <c r="AE4" s="71">
         <v>-1.3306257521871034E-2</v>
       </c>
-      <c r="AI4" s="69" t="str">
+      <c r="AF4" s="69" t="str">
         <f>'Tube L'!G2</f>
         <v>C9</v>
       </c>
-      <c r="AJ4" s="70">
+      <c r="AG4" s="70">
         <f>'Tube L'!F2</f>
         <v>1.7192995000000018</v>
       </c>
-      <c r="AK4" s="71">
+      <c r="AH4" s="71">
         <v>-1.8772590653531467E-2</v>
       </c>
-      <c r="AL4" s="69" t="str">
+      <c r="AI4" s="69" t="str">
         <f>'Tube M'!G2</f>
         <v>A1</v>
       </c>
-      <c r="AM4" s="70">
+      <c r="AJ4" s="70">
         <f>'Tube M'!F2</f>
         <v>1.7274678810000026</v>
       </c>
-      <c r="AN4" s="71">
+      <c r="AK4" s="71">
         <v>1.4702137864173308E-2</v>
       </c>
-      <c r="AO4" s="69" t="str">
+      <c r="AL4" s="69" t="str">
         <f>'Tube N'!G2</f>
         <v>G3</v>
       </c>
-      <c r="AP4" s="70">
+      <c r="AM4" s="70">
         <f>'Tube N'!F2</f>
         <v>1.7047111540000035</v>
       </c>
-      <c r="AQ4" s="71">
+      <c r="AN4" s="71">
         <v>1.5224739881171229E-2</v>
       </c>
-      <c r="AR4" s="69" t="str">
+      <c r="AO4" s="69" t="str">
         <f>'Tube O'!G2</f>
         <v>D6</v>
       </c>
-      <c r="AS4" s="70">
+      <c r="AP4" s="70">
         <f>'Tube O'!F2</f>
         <v>1.6961603070000013</v>
       </c>
-      <c r="AT4" s="71">
+      <c r="AQ4" s="71">
         <v>-2.8348128679534557E-2</v>
       </c>
-      <c r="AU4" s="69" t="str">
+      <c r="AR4" s="69" t="str">
         <f>'Tube P'!G2</f>
         <v>C9</v>
       </c>
-      <c r="AV4" s="70">
+      <c r="AS4" s="70">
         <f>'Tube P'!F2</f>
         <v>1.7183979730000019</v>
       </c>
-      <c r="AW4" s="71">
+      <c r="AT4" s="71">
         <v>-4.4743152942258078E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:46">
       <c r="A5" s="56">
         <v>2</v>
       </c>
@@ -21983,84 +21785,73 @@
         <v>4.869786341190032E-2</v>
       </c>
       <c r="AC5" s="72" t="str">
-        <f>'Tube J'!G3</f>
-        <v>H3</v>
-      </c>
-      <c r="AD5" s="70">
-        <f>'Tube J'!F3</f>
-        <v>1.7758225110000012</v>
-      </c>
-      <c r="AE5" s="74">
-        <v>-2.2744805687566292E-2</v>
-      </c>
-      <c r="AF5" s="72" t="str">
         <f>'Tube K'!G3</f>
         <v>C6</v>
       </c>
-      <c r="AG5" s="73">
+      <c r="AD5" s="73">
         <f>'Tube K'!F3</f>
         <v>1.7704133490000018</v>
       </c>
-      <c r="AH5" s="74">
+      <c r="AE5" s="74">
         <v>-2.0508800267029784E-2</v>
       </c>
-      <c r="AI5" s="72" t="str">
+      <c r="AF5" s="72" t="str">
         <f>'Tube L'!G3</f>
         <v>D9</v>
       </c>
-      <c r="AJ5" s="73">
+      <c r="AG5" s="73">
         <f>'Tube L'!F3</f>
         <v>1.7706592200000024</v>
       </c>
-      <c r="AK5" s="74">
+      <c r="AH5" s="74">
         <v>-2.0544099836460574E-2</v>
       </c>
-      <c r="AL5" s="72" t="str">
+      <c r="AI5" s="72" t="str">
         <f>'Tube M'!G3</f>
         <v>B1</v>
       </c>
-      <c r="AM5" s="73">
+      <c r="AJ5" s="73">
         <f>'Tube M'!F3</f>
         <v>1.7733638010000021</v>
       </c>
-      <c r="AN5" s="74">
+      <c r="AK5" s="74">
         <v>6.3186482923644705E-2</v>
       </c>
-      <c r="AO5" s="72" t="str">
+      <c r="AL5" s="72" t="str">
         <f>'Tube N'!G3</f>
         <v>H3</v>
       </c>
-      <c r="AP5" s="73">
+      <c r="AM5" s="73">
         <f>'Tube N'!F3</f>
         <v>1.7724622740000022</v>
       </c>
-      <c r="AQ5" s="74">
+      <c r="AN5" s="74">
         <v>0.12193627302478248</v>
       </c>
-      <c r="AR5" s="72" t="str">
+      <c r="AO5" s="72" t="str">
         <f>'Tube O'!G3</f>
         <v>C6</v>
       </c>
-      <c r="AS5" s="73">
+      <c r="AP5" s="73">
         <f>'Tube O'!F3</f>
         <v>1.7715607470000023</v>
       </c>
-      <c r="AT5" s="74">
+      <c r="AQ5" s="74">
         <v>-1.8810484504165701E-2</v>
       </c>
-      <c r="AU5" s="72" t="str">
+      <c r="AR5" s="72" t="str">
         <f>'Tube P'!G3</f>
         <v>D9</v>
       </c>
-      <c r="AV5" s="73">
+      <c r="AS5" s="73">
         <f>'Tube P'!F3</f>
         <v>1.7708504530000031</v>
       </c>
-      <c r="AW5" s="74">
+      <c r="AT5" s="74">
         <v>-3.9781679560703477E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:46">
       <c r="A6" s="56">
         <v>3</v>
       </c>
@@ -22164,84 +21955,73 @@
         <v>2.033399719090018E-3</v>
       </c>
       <c r="AC6" s="72" t="str">
-        <f>'Tube J'!G4</f>
-        <v>H4</v>
-      </c>
-      <c r="AD6" s="70">
-        <f>'Tube J'!F4</f>
-        <v>1.7681731910000025</v>
-      </c>
-      <c r="AE6" s="74">
-        <v>-2.1746969907379024E-2</v>
-      </c>
-      <c r="AF6" s="72" t="str">
         <f>'Tube K'!G4</f>
         <v>B6</v>
       </c>
-      <c r="AG6" s="73">
+      <c r="AD6" s="73">
         <f>'Tube K'!F4</f>
         <v>1.7660423090000013</v>
       </c>
-      <c r="AH6" s="74">
+      <c r="AE6" s="74">
         <v>7.7684855964655908E-3</v>
       </c>
-      <c r="AI6" s="72" t="str">
+      <c r="AF6" s="72" t="str">
         <f>'Tube L'!G4</f>
         <v>E9</v>
       </c>
-      <c r="AJ6" s="73">
+      <c r="AG6" s="73">
         <f>'Tube L'!F4</f>
         <v>1.7662881800000001</v>
       </c>
-      <c r="AK6" s="74">
+      <c r="AH6" s="74">
         <v>-1.0016522353316815E-2</v>
       </c>
-      <c r="AL6" s="72" t="str">
+      <c r="AI6" s="72" t="str">
         <f>'Tube M'!G4</f>
         <v>C1</v>
       </c>
-      <c r="AM6" s="73">
+      <c r="AJ6" s="73">
         <f>'Tube M'!F4</f>
         <v>1.7668072410000004</v>
       </c>
-      <c r="AN6" s="74">
+      <c r="AK6" s="74">
         <v>4.4851865026893256E-2</v>
       </c>
-      <c r="AO6" s="72" t="str">
+      <c r="AL6" s="72" t="str">
         <f>'Tube N'!G4</f>
         <v>H4</v>
       </c>
-      <c r="AP6" s="73">
+      <c r="AM6" s="73">
         <f>'Tube N'!F4</f>
         <v>1.7669984740000011</v>
       </c>
-      <c r="AQ6" s="74">
+      <c r="AN6" s="74">
         <v>0.48680306668578432</v>
       </c>
-      <c r="AR6" s="72" t="str">
+      <c r="AO6" s="72" t="str">
         <f>'Tube O'!G4</f>
         <v>B6</v>
       </c>
-      <c r="AS6" s="73">
+      <c r="AP6" s="73">
         <f>'Tube O'!F4</f>
         <v>1.7684737000000013</v>
       </c>
-      <c r="AT6" s="74">
+      <c r="AQ6" s="74">
         <v>6.7536811431441135E-2</v>
       </c>
-      <c r="AU6" s="72" t="str">
+      <c r="AR6" s="72" t="str">
         <f>'Tube P'!G4</f>
         <v>E9</v>
       </c>
-      <c r="AV6" s="73">
+      <c r="AS6" s="73">
         <f>'Tube P'!F4</f>
         <v>1.7664794130000008</v>
       </c>
-      <c r="AW6" s="74">
+      <c r="AT6" s="74">
         <v>-2.1652860706683524E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:46">
       <c r="A7" s="56">
         <v>4</v>
       </c>
@@ -22345,84 +22125,73 @@
         <v>1.2523313174823539E-2</v>
       </c>
       <c r="AC7" s="72" t="str">
-        <f>'Tube J'!G5</f>
-        <v>G4</v>
-      </c>
-      <c r="AD7" s="70">
-        <f>'Tube J'!F5</f>
-        <v>1.7616166310000008</v>
-      </c>
-      <c r="AE7" s="74">
-        <v>-3.069589655491865E-2</v>
-      </c>
-      <c r="AF7" s="72" t="str">
         <f>'Tube K'!G5</f>
         <v>A6</v>
       </c>
-      <c r="AG7" s="73">
+      <c r="AD7" s="73">
         <f>'Tube K'!F5</f>
         <v>1.7607697420000008</v>
       </c>
-      <c r="AH7" s="74">
+      <c r="AE7" s="74">
         <v>2.9126642796388272E-2</v>
       </c>
-      <c r="AI7" s="72" t="str">
+      <c r="AF7" s="72" t="str">
         <f>'Tube L'!G5</f>
         <v>F9</v>
       </c>
-      <c r="AJ7" s="73">
+      <c r="AG7" s="73">
         <f>'Tube L'!F5</f>
         <v>1.7608243800000007</v>
       </c>
-      <c r="AK7" s="74">
+      <c r="AH7" s="74">
         <v>4.0619630488657625E-2</v>
       </c>
-      <c r="AL7" s="72" t="str">
+      <c r="AI7" s="72" t="str">
         <f>'Tube M'!G5</f>
         <v>D1</v>
       </c>
-      <c r="AM7" s="73">
+      <c r="AJ7" s="73">
         <f>'Tube M'!F5</f>
         <v>1.7602506810000005</v>
       </c>
-      <c r="AN7" s="74">
+      <c r="AK7" s="74">
         <v>0.13345037046282857</v>
       </c>
-      <c r="AO7" s="72" t="str">
+      <c r="AL7" s="72" t="str">
         <f>'Tube N'!G5</f>
         <v>G4</v>
       </c>
-      <c r="AP7" s="73">
+      <c r="AM7" s="73">
         <f>'Tube N'!F5</f>
         <v>1.7604419140000012</v>
       </c>
-      <c r="AQ7" s="74">
+      <c r="AN7" s="74">
         <v>1.3380938965633746</v>
       </c>
-      <c r="AR7" s="72" t="str">
+      <c r="AO7" s="72" t="str">
         <f>'Tube O'!G5</f>
         <v>A6</v>
       </c>
-      <c r="AS7" s="73">
+      <c r="AP7" s="73">
         <f>'Tube O'!F5</f>
         <v>1.7608243800000007</v>
       </c>
-      <c r="AT7" s="74">
+      <c r="AQ7" s="74">
         <v>0.24991663297464087</v>
       </c>
-      <c r="AU7" s="72" t="str">
+      <c r="AR7" s="72" t="str">
         <f>'Tube P'!G5</f>
         <v>F9</v>
       </c>
-      <c r="AV7" s="73">
+      <c r="AS7" s="73">
         <f>'Tube P'!F5</f>
         <v>1.7610156130000014</v>
       </c>
-      <c r="AW7" s="74">
+      <c r="AT7" s="74">
         <v>4.9404213759198429E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:46">
       <c r="A8" s="56">
         <v>5</v>
       </c>
@@ -22525,85 +22294,74 @@
       <c r="AB8" s="74">
         <v>0.18051369372432502</v>
       </c>
-      <c r="AC8" s="109" t="str">
-        <f>'Tube J'!G6</f>
-        <v>F4</v>
-      </c>
-      <c r="AD8" s="70">
-        <f>'Tube J'!F6</f>
-        <v>1.7563440640000021</v>
-      </c>
-      <c r="AE8" s="110">
-        <v>4.3911836393426142E-2</v>
-      </c>
-      <c r="AF8" s="72" t="str">
+      <c r="AC8" s="72" t="str">
         <f>'Tube K'!G6</f>
         <v>A7</v>
       </c>
-      <c r="AG8" s="73">
+      <c r="AD8" s="73">
         <f>'Tube K'!F6</f>
         <v>1.7531204220000021</v>
       </c>
-      <c r="AH8" s="74">
+      <c r="AE8" s="74">
         <v>0.17180816000110699</v>
       </c>
-      <c r="AI8" s="72" t="str">
+      <c r="AF8" s="72" t="str">
         <f>'Tube L'!G6</f>
         <v>G9</v>
       </c>
-      <c r="AJ8" s="73">
+      <c r="AG8" s="73">
         <f>'Tube L'!F6</f>
         <v>1.7542678200000026</v>
       </c>
-      <c r="AK8" s="74">
+      <c r="AH8" s="74">
         <v>0.52518141383538175</v>
       </c>
-      <c r="AL8" s="72" t="str">
+      <c r="AI8" s="72" t="str">
         <f>'Tube M'!G6</f>
         <v>E1</v>
       </c>
-      <c r="AM8" s="73">
+      <c r="AJ8" s="73">
         <f>'Tube M'!F6</f>
         <v>1.7536941210000023</v>
       </c>
-      <c r="AN8" s="74">
+      <c r="AK8" s="74">
         <v>0.47492969241983457</v>
       </c>
-      <c r="AO8" s="72" t="str">
+      <c r="AL8" s="72" t="str">
         <f>'Tube N'!G6</f>
         <v>F4</v>
       </c>
-      <c r="AP8" s="73">
+      <c r="AM8" s="73">
         <f>'Tube N'!F6</f>
         <v>1.7527925940000024</v>
       </c>
-      <c r="AQ8" s="74">
+      <c r="AN8" s="74">
         <v>2.0747339542215109</v>
       </c>
-      <c r="AR8" s="72" t="str">
+      <c r="AO8" s="72" t="str">
         <f>'Tube O'!G6</f>
         <v>A7</v>
       </c>
-      <c r="AS8" s="73">
+      <c r="AP8" s="73">
         <f>'Tube O'!F6</f>
         <v>1.7542678200000026</v>
       </c>
-      <c r="AT8" s="74">
+      <c r="AQ8" s="74">
         <v>0.98431929103131865</v>
       </c>
-      <c r="AU8" s="72" t="str">
+      <c r="AR8" s="72" t="str">
         <f>'Tube P'!G6</f>
         <v>G9</v>
       </c>
-      <c r="AV8" s="73">
+      <c r="AS8" s="73">
         <f>'Tube P'!F6</f>
         <v>1.7533662930000027</v>
       </c>
-      <c r="AW8" s="74">
+      <c r="AT8" s="74">
         <v>0.27929987483596419</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:46">
       <c r="A9" s="56">
         <v>6</v>
       </c>
@@ -22706,85 +22464,74 @@
       <c r="AB9" s="74">
         <v>0.56496093986112872</v>
       </c>
-      <c r="AC9" s="109" t="str">
-        <f>'Tube J'!G7</f>
-        <v>E4</v>
-      </c>
-      <c r="AD9" s="70">
-        <f>'Tube J'!F7</f>
-        <v>1.7497875040000022</v>
-      </c>
-      <c r="AE9" s="110">
-        <v>0.17726908426687879</v>
-      </c>
-      <c r="AF9" s="72" t="str">
+      <c r="AC9" s="72" t="str">
         <f>'Tube K'!G7</f>
         <v>B7</v>
       </c>
-      <c r="AG9" s="73">
+      <c r="AD9" s="73">
         <f>'Tube K'!F7</f>
         <v>1.7467550950000028</v>
       </c>
-      <c r="AH9" s="74">
+      <c r="AE9" s="74">
         <v>0.43682661021063929</v>
       </c>
-      <c r="AI9" s="72" t="str">
+      <c r="AF9" s="72" t="str">
         <f>'Tube L'!G7</f>
         <v>H9</v>
       </c>
-      <c r="AJ9" s="73">
+      <c r="AG9" s="73">
         <f>'Tube L'!F7</f>
         <v>1.7477112600000027</v>
       </c>
-      <c r="AK9" s="74">
+      <c r="AH9" s="74">
         <v>1.3054778667218732</v>
       </c>
-      <c r="AL9" s="72" t="str">
+      <c r="AI9" s="72" t="str">
         <f>'Tube M'!G7</f>
         <v>F1</v>
       </c>
-      <c r="AM9" s="73">
+      <c r="AJ9" s="73">
         <f>'Tube M'!F7</f>
         <v>1.7471375610000024</v>
       </c>
-      <c r="AN9" s="74">
+      <c r="AK9" s="74">
         <v>1.5686088898700881</v>
       </c>
-      <c r="AO9" s="72" t="str">
+      <c r="AL9" s="72" t="str">
         <f>'Tube N'!G7</f>
         <v>E4</v>
       </c>
-      <c r="AP9" s="73">
+      <c r="AM9" s="73">
         <f>'Tube N'!F7</f>
         <v>1.7462360340000007</v>
       </c>
-      <c r="AQ9" s="74">
+      <c r="AN9" s="74">
         <v>3.5556387670298242</v>
       </c>
-      <c r="AR9" s="72" t="str">
+      <c r="AO9" s="72" t="str">
         <f>'Tube O'!G7</f>
         <v>B7</v>
       </c>
-      <c r="AS9" s="73">
+      <c r="AP9" s="73">
         <f>'Tube O'!F7</f>
         <v>1.7466185000000003</v>
       </c>
-      <c r="AT9" s="74">
+      <c r="AQ9" s="74">
         <v>2.3134210534842392</v>
       </c>
-      <c r="AU9" s="72" t="str">
+      <c r="AR9" s="72" t="str">
         <f>'Tube P'!G7</f>
         <v>H9</v>
       </c>
-      <c r="AV9" s="73">
+      <c r="AS9" s="73">
         <f>'Tube P'!F7</f>
         <v>1.7479024930000033</v>
       </c>
-      <c r="AW9" s="74">
+      <c r="AT9" s="74">
         <v>0.7034493623797351</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:46">
       <c r="A10" s="56">
         <v>7</v>
       </c>
@@ -22887,85 +22634,74 @@
       <c r="AB10" s="74">
         <v>1.6562602222431932</v>
       </c>
-      <c r="AC10" s="109" t="str">
-        <f>'Tube J'!G8</f>
-        <v>D4</v>
-      </c>
-      <c r="AD10" s="70">
-        <f>'Tube J'!F8</f>
-        <v>1.7619990970000003</v>
-      </c>
-      <c r="AE10" s="110">
-        <v>0.68477902703551463</v>
-      </c>
-      <c r="AF10" s="72" t="str">
+      <c r="AC10" s="72" t="str">
         <f>'Tube K'!G8</f>
         <v>C7</v>
       </c>
-      <c r="AG10" s="73">
+      <c r="AD10" s="73">
         <f>'Tube K'!F8</f>
         <v>1.7401985350000011</v>
       </c>
-      <c r="AH10" s="74">
+      <c r="AE10" s="74">
         <v>1.3112103265513564</v>
       </c>
-      <c r="AI10" s="72" t="str">
+      <c r="AF10" s="72" t="str">
         <f>'Tube L'!G8</f>
         <v>H10</v>
       </c>
-      <c r="AJ10" s="73">
+      <c r="AG10" s="73">
         <f>'Tube L'!F8</f>
         <v>1.7411547000000009</v>
       </c>
-      <c r="AK10" s="75">
+      <c r="AH10" s="75">
         <v>1.9497283100690577</v>
       </c>
-      <c r="AL10" s="72" t="str">
+      <c r="AI10" s="72" t="str">
         <f>'Tube M'!G8</f>
         <v>G1</v>
       </c>
-      <c r="AM10" s="73">
+      <c r="AJ10" s="73">
         <f>'Tube M'!F8</f>
         <v>1.7416737610000013</v>
       </c>
-      <c r="AN10" s="74">
+      <c r="AK10" s="74">
         <v>3.8685849537547372</v>
       </c>
-      <c r="AO10" s="72" t="str">
+      <c r="AL10" s="72" t="str">
         <f>'Tube N'!G8</f>
         <v>D4</v>
       </c>
-      <c r="AP10" s="73">
+      <c r="AM10" s="73">
         <f>'Tube N'!F8</f>
         <v>1.7407722340000014</v>
       </c>
-      <c r="AQ10" s="74">
+      <c r="AN10" s="74">
         <v>5.5498797152488537</v>
       </c>
-      <c r="AR10" s="72" t="str">
+      <c r="AO10" s="72" t="str">
         <f>'Tube O'!G8</f>
         <v>C7</v>
       </c>
-      <c r="AS10" s="73">
+      <c r="AP10" s="73">
         <f>'Tube O'!F8</f>
         <v>1.7411547000000009</v>
       </c>
-      <c r="AT10" s="74">
+      <c r="AQ10" s="74">
         <v>3.4880804138453461</v>
       </c>
-      <c r="AU10" s="72" t="str">
+      <c r="AR10" s="72" t="str">
         <f>'Tube P'!G8</f>
         <v>H10</v>
       </c>
-      <c r="AV10" s="73">
+      <c r="AS10" s="73">
         <f>'Tube P'!F8</f>
         <v>1.7413459330000016</v>
       </c>
-      <c r="AW10" s="75">
+      <c r="AT10" s="75">
         <v>1.3897911787239454</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:46">
       <c r="A11" s="56">
         <v>8</v>
       </c>
@@ -23067,85 +22803,74 @@
       <c r="AB11" s="74">
         <v>4.0622502134945657</v>
       </c>
-      <c r="AC11" s="109" t="str">
-        <f>'Tube J'!G9</f>
-        <v>C4</v>
-      </c>
-      <c r="AD11" s="70">
-        <f>'Tube J'!F9</f>
-        <v>1.737958377</v>
-      </c>
-      <c r="AE11" s="110">
-        <v>1.1653297508468299</v>
-      </c>
-      <c r="AF11" s="72" t="str">
+      <c r="AC11" s="72" t="str">
         <f>'Tube K'!G9</f>
         <v>D7</v>
       </c>
-      <c r="AG11" s="73">
+      <c r="AD11" s="73">
         <f>'Tube K'!F9</f>
         <v>1.7336419750000012</v>
       </c>
-      <c r="AH11" s="74">
+      <c r="AE11" s="74">
         <v>3.4525502047068968</v>
       </c>
-      <c r="AI11" s="72" t="str">
+      <c r="AF11" s="72" t="str">
         <f>'Tube L'!G9</f>
         <v>G10</v>
       </c>
-      <c r="AJ11" s="73">
+      <c r="AG11" s="73">
         <f>'Tube L'!F9</f>
         <v>1.7356909000000016</v>
       </c>
-      <c r="AK11" s="75">
+      <c r="AH11" s="75">
         <v>3.4293576676570763</v>
       </c>
-      <c r="AL11" s="72" t="str">
+      <c r="AI11" s="72" t="str">
         <f>'Tube M'!G9</f>
         <v>H1</v>
       </c>
-      <c r="AM11" s="73">
+      <c r="AJ11" s="73">
         <f>'Tube M'!F9</f>
         <v>1.7351172010000013</v>
       </c>
-      <c r="AN11" s="74">
+      <c r="AK11" s="74">
         <v>8.4205998751906517</v>
       </c>
-      <c r="AO11" s="72" t="str">
+      <c r="AL11" s="72" t="str">
         <f>'Tube N'!G9</f>
         <v>C4</v>
       </c>
-      <c r="AP11" s="73">
+      <c r="AM11" s="73">
         <f>'Tube N'!F9</f>
         <v>1.735308434000002</v>
       </c>
-      <c r="AQ11" s="74">
+      <c r="AN11" s="74">
         <v>8.14646368710447</v>
       </c>
-      <c r="AR11" s="72" t="str">
+      <c r="AO11" s="72" t="str">
         <f>'Tube O'!G9</f>
         <v>D7</v>
       </c>
-      <c r="AS11" s="73">
+      <c r="AP11" s="73">
         <f>'Tube O'!F9</f>
         <v>1.7356909000000016</v>
       </c>
-      <c r="AT11" s="74">
+      <c r="AQ11" s="74">
         <v>5.9006595991068087</v>
       </c>
-      <c r="AU11" s="72" t="str">
+      <c r="AR11" s="72" t="str">
         <f>'Tube P'!G9</f>
         <v>G10</v>
       </c>
-      <c r="AV11" s="73">
+      <c r="AS11" s="73">
         <f>'Tube P'!F9</f>
         <v>1.7358821330000023</v>
       </c>
-      <c r="AW11" s="75">
+      <c r="AT11" s="75">
         <v>3.5254495168872464</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:46">
       <c r="A12" s="56">
         <v>9</v>
       </c>
@@ -23248,85 +22973,74 @@
       <c r="AB12" s="74">
         <v>9.4634308887455152</v>
       </c>
-      <c r="AC12" s="109" t="str">
-        <f>'Tube J'!G10</f>
-        <v>B4</v>
-      </c>
-      <c r="AD12" s="70">
-        <f>'Tube J'!F10</f>
-        <v>1.7467004570000029</v>
-      </c>
-      <c r="AE12" s="110">
-        <v>1.0272573685676323</v>
-      </c>
-      <c r="AF12" s="72" t="str">
+      <c r="AC12" s="72" t="str">
         <f>'Tube K'!G10</f>
         <v>E7</v>
       </c>
-      <c r="AG12" s="73">
+      <c r="AD12" s="73">
         <f>'Tube K'!F10</f>
         <v>1.7283694080000025</v>
       </c>
-      <c r="AH12" s="74">
+      <c r="AE12" s="74">
         <v>11.432153270319313</v>
       </c>
-      <c r="AI12" s="72" t="str">
+      <c r="AF12" s="72" t="str">
         <f>'Tube L'!G10</f>
         <v>F10</v>
       </c>
-      <c r="AJ12" s="73">
+      <c r="AG12" s="73">
         <f>'Tube L'!F10</f>
         <v>1.7291343400000017</v>
       </c>
-      <c r="AK12" s="75">
+      <c r="AH12" s="75">
         <v>6.5066160189663416</v>
       </c>
-      <c r="AL12" s="72" t="str">
+      <c r="AI12" s="72" t="str">
         <f>'Tube M'!G10</f>
         <v>H2</v>
       </c>
-      <c r="AM12" s="73">
+      <c r="AJ12" s="73">
         <f>'Tube M'!F10</f>
         <v>1.729653401000002</v>
       </c>
-      <c r="AN12" s="74">
+      <c r="AK12" s="74">
         <v>14.81633132361892</v>
       </c>
-      <c r="AO12" s="72" t="str">
+      <c r="AL12" s="72" t="str">
         <f>'Tube N'!G10</f>
         <v>B4</v>
       </c>
-      <c r="AP12" s="73">
+      <c r="AM12" s="73">
         <f>'Tube N'!F10</f>
         <v>1.7300358670000016</v>
       </c>
-      <c r="AQ12" s="74">
+      <c r="AN12" s="74">
         <v>13.248461262565771</v>
       </c>
-      <c r="AR12" s="72" t="str">
+      <c r="AO12" s="72" t="str">
         <f>'Tube O'!G10</f>
         <v>E7</v>
       </c>
-      <c r="AS12" s="73">
+      <c r="AP12" s="73">
         <f>'Tube O'!F10</f>
         <v>1.7302271000000022</v>
       </c>
-      <c r="AT12" s="74">
+      <c r="AQ12" s="74">
         <v>11.345868321399378</v>
       </c>
-      <c r="AU12" s="72" t="str">
+      <c r="AR12" s="72" t="str">
         <f>'Tube P'!G10</f>
         <v>F10</v>
       </c>
-      <c r="AV12" s="73">
+      <c r="AS12" s="73">
         <f>'Tube P'!F10</f>
         <v>1.7293255730000023</v>
       </c>
-      <c r="AW12" s="75">
+      <c r="AT12" s="75">
         <v>10.28105064029954</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:46">
       <c r="A13" s="56">
         <v>10</v>
       </c>
@@ -23430,84 +23144,73 @@
         <v>13.894035924079773</v>
       </c>
       <c r="AC13" s="72" t="str">
-        <f>'Tube J'!G11</f>
-        <v>A4</v>
-      </c>
-      <c r="AD13" s="70">
-        <f>'Tube J'!F11</f>
-        <v>1.7326858100000013</v>
-      </c>
-      <c r="AE13" s="74">
-        <v>9.1297521523685372</v>
-      </c>
-      <c r="AF13" s="72" t="str">
         <f>'Tube K'!G11</f>
         <v>F7</v>
       </c>
-      <c r="AG13" s="73">
+      <c r="AD13" s="73">
         <f>'Tube K'!F11</f>
         <v>1.7229056080000014</v>
       </c>
-      <c r="AH13" s="74">
+      <c r="AE13" s="74">
         <v>14.920287367280102</v>
       </c>
-      <c r="AI13" s="72" t="str">
+      <c r="AF13" s="72" t="str">
         <f>'Tube L'!G11</f>
         <v>E10</v>
       </c>
-      <c r="AJ13" s="73">
+      <c r="AG13" s="73">
         <f>'Tube L'!F11</f>
         <v>1.7236705400000005</v>
       </c>
-      <c r="AK13" s="74">
+      <c r="AH13" s="74">
         <v>13.337302438515778</v>
       </c>
-      <c r="AL13" s="72" t="str">
+      <c r="AI13" s="72" t="str">
         <f>'Tube M'!G11</f>
         <v>G2</v>
       </c>
-      <c r="AM13" s="73">
+      <c r="AJ13" s="73">
         <f>'Tube M'!F11</f>
         <v>1.7241896010000008</v>
       </c>
-      <c r="AN13" s="74">
+      <c r="AK13" s="74">
         <v>17.292750188722547</v>
       </c>
-      <c r="AO13" s="72" t="str">
+      <c r="AL13" s="72" t="str">
         <f>'Tube N'!G11</f>
         <v>A4</v>
       </c>
-      <c r="AP13" s="73">
+      <c r="AM13" s="73">
         <f>'Tube N'!F11</f>
         <v>1.7234793069999998</v>
       </c>
-      <c r="AQ13" s="74">
+      <c r="AN13" s="74">
         <v>15.97654093038139</v>
       </c>
-      <c r="AR13" s="72" t="str">
+      <c r="AO13" s="72" t="str">
         <f>'Tube O'!G11</f>
         <v>F7</v>
       </c>
-      <c r="AS13" s="73">
+      <c r="AP13" s="73">
         <f>'Tube O'!F11</f>
         <v>1.7236705400000005</v>
       </c>
-      <c r="AT13" s="74">
+      <c r="AQ13" s="74">
         <v>14.621005651178303</v>
       </c>
-      <c r="AU13" s="72" t="str">
+      <c r="AR13" s="72" t="str">
         <f>'Tube P'!G11</f>
         <v>E10</v>
       </c>
-      <c r="AV13" s="73">
+      <c r="AS13" s="73">
         <f>'Tube P'!F11</f>
         <v>1.7238617730000012</v>
       </c>
-      <c r="AW13" s="74">
+      <c r="AT13" s="74">
         <v>14.498673624841553</v>
       </c>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:46">
       <c r="A14" s="56">
         <v>11</v>
       </c>
@@ -23611,84 +23314,73 @@
         <v>9.3380302060060725</v>
       </c>
       <c r="AC14" s="72" t="str">
-        <f>'Tube J'!G12</f>
-        <v>A5</v>
-      </c>
-      <c r="AD14" s="70">
-        <f>'Tube J'!F12</f>
-        <v>1.7195726899999997</v>
-      </c>
-      <c r="AE14" s="74">
-        <v>12.790632613549747</v>
-      </c>
-      <c r="AF14" s="72" t="str">
         <f>'Tube K'!G12</f>
         <v>G7</v>
       </c>
-      <c r="AG14" s="73">
+      <c r="AD14" s="73">
         <f>'Tube K'!F12</f>
         <v>1.7163490480000014</v>
       </c>
-      <c r="AH14" s="74">
+      <c r="AE14" s="74">
         <v>11.6616887975174</v>
       </c>
-      <c r="AI14" s="72" t="str">
+      <c r="AF14" s="72" t="str">
         <f>'Tube L'!G12</f>
         <v>D10</v>
       </c>
-      <c r="AJ14" s="73">
+      <c r="AG14" s="73">
         <f>'Tube L'!F12</f>
         <v>1.7171139800000006</v>
       </c>
-      <c r="AK14" s="76">
+      <c r="AH14" s="76">
         <v>13.400413060411545</v>
       </c>
-      <c r="AL14" s="72" t="str">
+      <c r="AI14" s="72" t="str">
         <f>'Tube M'!G12</f>
         <v>F2</v>
       </c>
-      <c r="AM14" s="73">
+      <c r="AJ14" s="73">
         <f>'Tube M'!F12</f>
         <v>1.7176330410000009</v>
       </c>
-      <c r="AN14" s="74">
+      <c r="AK14" s="74">
         <v>13.25429560884875</v>
       </c>
-      <c r="AO14" s="72" t="str">
+      <c r="AL14" s="72" t="str">
         <f>'Tube N'!G12</f>
         <v>A5</v>
       </c>
-      <c r="AP14" s="73">
+      <c r="AM14" s="73">
         <f>'Tube N'!F12</f>
         <v>1.7202010270000017</v>
       </c>
-      <c r="AQ14" s="74">
+      <c r="AN14" s="74">
         <v>11.844444225998366</v>
       </c>
-      <c r="AR14" s="72" t="str">
+      <c r="AO14" s="72" t="str">
         <f>'Tube O'!G12</f>
         <v>G7</v>
       </c>
-      <c r="AS14" s="73">
+      <c r="AP14" s="73">
         <f>'Tube O'!F12</f>
         <v>1.7182067400000012</v>
       </c>
-      <c r="AT14" s="74">
+      <c r="AQ14" s="74">
         <v>15.661453605343306</v>
       </c>
-      <c r="AU14" s="72" t="str">
+      <c r="AR14" s="72" t="str">
         <f>'Tube P'!G12</f>
         <v>D10</v>
       </c>
-      <c r="AV14" s="73">
+      <c r="AS14" s="73">
         <f>'Tube P'!F12</f>
         <v>1.7183979730000019</v>
       </c>
-      <c r="AW14" s="76">
+      <c r="AT14" s="76">
         <v>10.279664980968116</v>
       </c>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:46">
       <c r="A15" s="56">
         <v>12</v>
       </c>
@@ -23792,84 +23484,73 @@
         <v>6.5039401130602323</v>
       </c>
       <c r="AC15" s="72" t="str">
-        <f>'Tube J'!G13</f>
-        <v>B5</v>
-      </c>
-      <c r="AD15" s="70">
-        <f>'Tube J'!F13</f>
-        <v>1.714300123000001</v>
-      </c>
-      <c r="AE15" s="74">
-        <v>8.6880382036748482</v>
-      </c>
-      <c r="AF15" s="72" t="str">
         <f>'Tube K'!G13</f>
         <v>H7</v>
       </c>
-      <c r="AG15" s="73">
+      <c r="AD15" s="73">
         <f>'Tube K'!F13</f>
         <v>1.7108852480000021</v>
       </c>
-      <c r="AH15" s="74">
+      <c r="AE15" s="74">
         <v>5.0824571249641481</v>
       </c>
-      <c r="AI15" s="72" t="str">
+      <c r="AF15" s="72" t="str">
         <f>'Tube L'!G13</f>
         <v>C10</v>
       </c>
-      <c r="AJ15" s="73">
+      <c r="AG15" s="73">
         <f>'Tube L'!F13</f>
         <v>1.7118414130000019</v>
       </c>
-      <c r="AK15" s="76">
+      <c r="AH15" s="76">
         <v>8.9004058730514757</v>
       </c>
-      <c r="AL15" s="72" t="str">
+      <c r="AI15" s="72" t="str">
         <f>'Tube M'!G13</f>
         <v>E2</v>
       </c>
-      <c r="AM15" s="73">
+      <c r="AJ15" s="73">
         <f>'Tube M'!F13</f>
         <v>1.7110764810000028</v>
       </c>
-      <c r="AN15" s="74">
+      <c r="AK15" s="74">
         <v>8.0162178469532321</v>
       </c>
-      <c r="AO15" s="72" t="str">
+      <c r="AL15" s="72" t="str">
         <f>'Tube N'!G13</f>
         <v>B5</v>
       </c>
-      <c r="AP15" s="73">
+      <c r="AM15" s="73">
         <f>'Tube N'!F13</f>
         <v>1.7136444670000017</v>
       </c>
-      <c r="AQ15" s="74">
+      <c r="AN15" s="74">
         <v>8.3655654476161327</v>
       </c>
-      <c r="AR15" s="72" t="str">
+      <c r="AO15" s="72" t="str">
         <f>'Tube O'!G13</f>
         <v>H7</v>
       </c>
-      <c r="AS15" s="73">
+      <c r="AP15" s="73">
         <f>'Tube O'!F13</f>
         <v>1.7127429400000018</v>
       </c>
-      <c r="AT15" s="74">
+      <c r="AQ15" s="74">
         <v>11.377615105143439</v>
       </c>
-      <c r="AU15" s="72" t="str">
+      <c r="AR15" s="72" t="str">
         <f>'Tube P'!G13</f>
         <v>C10</v>
       </c>
-      <c r="AV15" s="73">
+      <c r="AS15" s="73">
         <f>'Tube P'!F13</f>
         <v>1.7118414130000019</v>
       </c>
-      <c r="AW15" s="76">
+      <c r="AT15" s="76">
         <v>2.6104943278541106</v>
       </c>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:46">
       <c r="A16" s="56">
         <v>13</v>
       </c>
@@ -23973,84 +23654,73 @@
         <v>1.9953174219599272</v>
       </c>
       <c r="AC16" s="72" t="str">
-        <f>'Tube J'!G14</f>
-        <v>C5</v>
-      </c>
-      <c r="AD16" s="70">
-        <f>'Tube J'!F14</f>
-        <v>1.7088363230000017</v>
-      </c>
-      <c r="AE16" s="74">
-        <v>3.4817869109138084</v>
-      </c>
-      <c r="AF16" s="72" t="str">
         <f>'Tube K'!G14</f>
         <v>H8</v>
       </c>
-      <c r="AG16" s="73">
+      <c r="AD16" s="73">
         <f>'Tube K'!F14</f>
         <v>1.7065142080000015</v>
       </c>
-      <c r="AH16" s="74">
+      <c r="AE16" s="74">
         <v>2.5584160877238573</v>
       </c>
-      <c r="AI16" s="72" t="str">
+      <c r="AF16" s="72" t="str">
         <f>'Tube L'!G14</f>
         <v>B10</v>
       </c>
-      <c r="AJ16" s="73">
+      <c r="AG16" s="73">
         <f>'Tube L'!F14</f>
         <v>1.7063776130000026</v>
       </c>
-      <c r="AK16" s="76">
+      <c r="AH16" s="76">
         <v>4.5590228775748303</v>
       </c>
-      <c r="AL16" s="72" t="str">
+      <c r="AI16" s="72" t="str">
         <f>'Tube M'!G14</f>
         <v>D2</v>
       </c>
-      <c r="AM16" s="73">
+      <c r="AJ16" s="73">
         <f>'Tube M'!F14</f>
         <v>1.7099837210000022</v>
       </c>
-      <c r="AN16" s="74">
+      <c r="AK16" s="74">
         <v>3.5176775412692911</v>
       </c>
-      <c r="AO16" s="72" t="str">
+      <c r="AL16" s="72" t="str">
         <f>'Tube N'!G14</f>
         <v>C5</v>
       </c>
-      <c r="AP16" s="73">
+      <c r="AM16" s="73">
         <f>'Tube N'!F14</f>
         <v>1.7070879070000018</v>
       </c>
-      <c r="AQ16" s="74">
+      <c r="AN16" s="74">
         <v>3.5771665663069592</v>
       </c>
-      <c r="AR16" s="72" t="str">
+      <c r="AO16" s="72" t="str">
         <f>'Tube O'!G14</f>
         <v>H8</v>
       </c>
-      <c r="AS16" s="73">
+      <c r="AP16" s="73">
         <f>'Tube O'!F14</f>
         <v>1.7072791400000025</v>
       </c>
-      <c r="AT16" s="74">
+      <c r="AQ16" s="74">
         <v>4.5533829483903459</v>
       </c>
-      <c r="AU16" s="72" t="str">
+      <c r="AR16" s="72" t="str">
         <f>'Tube P'!G14</f>
         <v>B10</v>
       </c>
-      <c r="AV16" s="73">
+      <c r="AS16" s="73">
         <f>'Tube P'!F14</f>
         <v>1.7065688460000032</v>
       </c>
-      <c r="AW16" s="76">
+      <c r="AT16" s="76">
         <v>0.73701625263782544</v>
       </c>
     </row>
-    <row r="17" spans="1:49">
+    <row r="17" spans="1:46">
       <c r="A17" s="56">
         <v>14</v>
       </c>
@@ -24154,84 +23824,73 @@
         <v>1.0023161533702638</v>
       </c>
       <c r="AC17" s="72" t="str">
-        <f>'Tube J'!G15</f>
-        <v>D5</v>
-      </c>
-      <c r="AD17" s="70">
-        <f>'Tube J'!F15</f>
-        <v>1.7011870029999994</v>
-      </c>
-      <c r="AE17" s="74">
-        <v>1.4925442748630395</v>
-      </c>
-      <c r="AF17" s="72" t="str">
         <f>'Tube K'!G15</f>
         <v>G8</v>
       </c>
-      <c r="AG17" s="73">
+      <c r="AD17" s="73">
         <f>'Tube K'!F15</f>
         <v>1.6990561209999999</v>
       </c>
-      <c r="AH17" s="74">
+      <c r="AE17" s="74">
         <v>1.1294502939287847</v>
       </c>
-      <c r="AI17" s="72" t="str">
+      <c r="AF17" s="72" t="str">
         <f>'Tube L'!G15</f>
         <v>A10</v>
       </c>
-      <c r="AJ17" s="73">
+      <c r="AG17" s="73">
         <f>'Tube L'!F15</f>
         <v>1.6998210530000009</v>
       </c>
-      <c r="AK17" s="74">
+      <c r="AH17" s="74">
         <v>1.8282603961800705</v>
       </c>
-      <c r="AL17" s="72" t="str">
+      <c r="AI17" s="72" t="str">
         <f>'Tube M'!G15</f>
         <v>C2</v>
       </c>
-      <c r="AM17" s="73">
+      <c r="AJ17" s="73">
         <f>'Tube M'!F15</f>
         <v>1.7001488810000005</v>
       </c>
-      <c r="AN17" s="74">
+      <c r="AK17" s="74">
         <v>1.7447730542507918</v>
       </c>
-      <c r="AO17" s="72" t="str">
+      <c r="AL17" s="72" t="str">
         <f>'Tube N'!G15</f>
         <v>D5</v>
       </c>
-      <c r="AP17" s="73">
+      <c r="AM17" s="73">
         <f>'Tube N'!F15</f>
         <v>1.7016241070000007</v>
       </c>
-      <c r="AQ17" s="74">
+      <c r="AN17" s="74">
         <v>1.8467678326212711</v>
       </c>
-      <c r="AR17" s="72" t="str">
+      <c r="AO17" s="72" t="str">
         <f>'Tube O'!G15</f>
         <v>G8</v>
       </c>
-      <c r="AS17" s="73">
+      <c r="AP17" s="73">
         <f>'Tube O'!F15</f>
         <v>1.7007225800000008</v>
       </c>
-      <c r="AT17" s="74">
+      <c r="AQ17" s="74">
         <v>1.9541623903303273</v>
       </c>
-      <c r="AU17" s="72" t="str">
+      <c r="AR17" s="72" t="str">
         <f>'Tube P'!G15</f>
         <v>A10</v>
       </c>
-      <c r="AV17" s="73">
+      <c r="AS17" s="73">
         <f>'Tube P'!F15</f>
         <v>1.7011050460000003</v>
       </c>
-      <c r="AW17" s="74">
+      <c r="AT17" s="74">
         <v>0.41153011195458339</v>
       </c>
     </row>
-    <row r="18" spans="1:49">
+    <row r="18" spans="1:46">
       <c r="A18" s="56">
         <v>15</v>
       </c>
@@ -24335,84 +23994,73 @@
         <v>0.59468341834220828</v>
       </c>
       <c r="AC18" s="72" t="str">
-        <f>'Tube J'!G16</f>
-        <v>E5</v>
-      </c>
-      <c r="AD18" s="70">
-        <f>'Tube J'!F16</f>
-        <v>1.6946304430000012</v>
-      </c>
-      <c r="AE18" s="74">
-        <v>0.73640113105829552</v>
-      </c>
-      <c r="AF18" s="72" t="str">
         <f>'Tube K'!G16</f>
         <v>F8</v>
       </c>
-      <c r="AG18" s="73">
+      <c r="AD18" s="73">
         <f>'Tube K'!F16</f>
         <v>1.6946850810000011</v>
       </c>
-      <c r="AH18" s="74">
+      <c r="AE18" s="74">
         <v>0.6774963964524362</v>
       </c>
-      <c r="AI18" s="72" t="str">
+      <c r="AF18" s="72" t="str">
         <f>'Tube L'!G16</f>
         <v>A11</v>
       </c>
-      <c r="AJ18" s="73">
+      <c r="AG18" s="73">
         <f>'Tube L'!F16</f>
         <v>1.6943572530000015</v>
       </c>
-      <c r="AK18" s="74">
+      <c r="AH18" s="74">
         <v>1.0088363866594818</v>
       </c>
-      <c r="AL18" s="72" t="str">
+      <c r="AI18" s="72" t="str">
         <f>'Tube M'!G16</f>
         <v>B2</v>
       </c>
-      <c r="AM18" s="73">
+      <c r="AJ18" s="73">
         <f>'Tube M'!F16</f>
         <v>1.6935923210000006</v>
       </c>
-      <c r="AN18" s="74">
+      <c r="AK18" s="74">
         <v>0.96756092775874381</v>
       </c>
-      <c r="AO18" s="72" t="str">
+      <c r="AL18" s="72" t="str">
         <f>'Tube N'!G16</f>
         <v>E5</v>
       </c>
-      <c r="AP18" s="73">
+      <c r="AM18" s="73">
         <f>'Tube N'!F16</f>
         <v>1.6939747870000019</v>
       </c>
-      <c r="AQ18" s="74">
+      <c r="AN18" s="74">
         <v>1.011144818023834</v>
       </c>
-      <c r="AR18" s="72" t="str">
+      <c r="AO18" s="72" t="str">
         <f>'Tube O'!G16</f>
         <v>F8</v>
       </c>
-      <c r="AS18" s="73">
+      <c r="AP18" s="73">
         <f>'Tube O'!F16</f>
         <v>1.6952587800000014</v>
       </c>
-      <c r="AT18" s="74">
+      <c r="AQ18" s="74">
         <v>1.0133304734843103</v>
       </c>
-      <c r="AU18" s="72" t="str">
+      <c r="AR18" s="72" t="str">
         <f>'Tube P'!G16</f>
         <v>A11</v>
       </c>
-      <c r="AV18" s="73">
+      <c r="AS18" s="73">
         <f>'Tube P'!F16</f>
         <v>1.6947397190000011</v>
       </c>
-      <c r="AW18" s="74">
+      <c r="AT18" s="74">
         <v>0.99454273018992134</v>
       </c>
     </row>
-    <row r="19" spans="1:49">
+    <row r="19" spans="1:46">
       <c r="A19" s="56">
         <v>16</v>
       </c>
@@ -24516,84 +24164,73 @@
         <v>0.30542242106959722</v>
       </c>
       <c r="AC19" s="72" t="str">
-        <f>'Tube J'!G17</f>
-        <v>F5</v>
-      </c>
-      <c r="AD19" s="70">
-        <f>'Tube J'!F17</f>
-        <v>1.6891666430000019</v>
-      </c>
-      <c r="AE19" s="74">
-        <v>0.40619333424236964</v>
-      </c>
-      <c r="AF19" s="72" t="str">
         <f>'Tube K'!G17</f>
         <v>E8</v>
       </c>
-      <c r="AG19" s="73">
+      <c r="AD19" s="73">
         <f>'Tube K'!F17</f>
         <v>1.6881285210000012</v>
       </c>
-      <c r="AH19" s="74">
+      <c r="AE19" s="74">
         <v>0.42153897402091417</v>
       </c>
-      <c r="AI19" s="72" t="str">
+      <c r="AF19" s="72" t="str">
         <f>'Tube L'!G17</f>
         <v>B11</v>
       </c>
-      <c r="AJ19" s="73">
+      <c r="AG19" s="73">
         <f>'Tube L'!F17</f>
         <v>1.6878006930000016</v>
       </c>
-      <c r="AK19" s="74">
+      <c r="AH19" s="74">
         <v>0.50384949825866554</v>
       </c>
-      <c r="AL19" s="72" t="str">
+      <c r="AI19" s="72" t="str">
         <f>'Tube M'!G17</f>
         <v>A2</v>
       </c>
-      <c r="AM19" s="73">
+      <c r="AJ19" s="73">
         <f>'Tube M'!F17</f>
         <v>1.6881285210000012</v>
       </c>
-      <c r="AN19" s="74">
+      <c r="AK19" s="74">
         <v>0.58010849518820307</v>
       </c>
-      <c r="AO19" s="72" t="str">
+      <c r="AL19" s="72" t="str">
         <f>'Tube N'!G17</f>
         <v>F5</v>
       </c>
-      <c r="AP19" s="73">
+      <c r="AM19" s="73">
         <f>'Tube N'!F17</f>
         <v>1.6885109870000026</v>
       </c>
-      <c r="AQ19" s="74">
+      <c r="AN19" s="74">
         <v>0.57443247472007519</v>
       </c>
-      <c r="AR19" s="72" t="str">
+      <c r="AO19" s="72" t="str">
         <f>'Tube O'!G17</f>
         <v>E8</v>
       </c>
-      <c r="AS19" s="73">
+      <c r="AP19" s="73">
         <f>'Tube O'!F17</f>
         <v>1.6921717330000021</v>
       </c>
-      <c r="AT19" s="74">
+      <c r="AQ19" s="74">
         <v>0.42420890792620614</v>
       </c>
-      <c r="AU19" s="72" t="str">
+      <c r="AR19" s="72" t="str">
         <f>'Tube P'!G17</f>
         <v>B11</v>
       </c>
-      <c r="AV19" s="73">
+      <c r="AS19" s="73">
         <f>'Tube P'!F17</f>
         <v>1.6892759190000017</v>
       </c>
-      <c r="AW19" s="74">
+      <c r="AT19" s="74">
         <v>0.11907381158411545</v>
       </c>
     </row>
-    <row r="20" spans="1:49">
+    <row r="20" spans="1:46">
       <c r="A20" s="56">
         <v>17</v>
       </c>
@@ -24697,84 +24334,73 @@
         <v>0.16416767596994841</v>
       </c>
       <c r="AC20" s="72" t="str">
-        <f>'Tube J'!G18</f>
-        <v>G5</v>
-      </c>
-      <c r="AD20" s="70">
-        <f>'Tube J'!F18</f>
-        <v>1.6828013160000026</v>
-      </c>
-      <c r="AE20" s="74">
-        <v>0.21686418843300589</v>
-      </c>
-      <c r="AF20" s="72" t="str">
         <f>'Tube K'!G18</f>
         <v>D8</v>
       </c>
-      <c r="AG20" s="73">
+      <c r="AD20" s="73">
         <f>'Tube K'!F18</f>
         <v>1.6815719610000031</v>
       </c>
-      <c r="AH20" s="74">
+      <c r="AE20" s="74">
         <v>0.19900327875670809</v>
       </c>
-      <c r="AI20" s="72" t="str">
+      <c r="AF20" s="72" t="str">
         <f>'Tube L'!G18</f>
         <v>C11</v>
       </c>
-      <c r="AJ20" s="73">
+      <c r="AG20" s="73">
         <f>'Tube L'!F18</f>
         <v>1.6834296530000028</v>
       </c>
-      <c r="AK20" s="74">
+      <c r="AH20" s="74">
         <v>0.27837003103470986</v>
       </c>
-      <c r="AL20" s="72" t="str">
+      <c r="AI20" s="72" t="str">
         <f>'Tube M'!G18</f>
         <v>A3</v>
       </c>
-      <c r="AM20" s="73">
+      <c r="AJ20" s="73">
         <f>'Tube M'!F18</f>
         <v>1.681763194000002</v>
       </c>
-      <c r="AN20" s="74">
+      <c r="AK20" s="74">
         <v>0.30394969137950151</v>
       </c>
-      <c r="AO20" s="72" t="str">
+      <c r="AL20" s="72" t="str">
         <f>'Tube N'!G18</f>
         <v>G5</v>
       </c>
-      <c r="AP20" s="73">
+      <c r="AM20" s="73">
         <f>'Tube N'!F18</f>
         <v>1.6819544270000026</v>
       </c>
-      <c r="AQ20" s="74">
+      <c r="AN20" s="74">
         <v>0.43474865162407794</v>
       </c>
-      <c r="AR20" s="72" t="str">
+      <c r="AO20" s="72" t="str">
         <f>'Tube O'!G18</f>
         <v>D8</v>
       </c>
-      <c r="AS20" s="73">
+      <c r="AP20" s="73">
         <f>'Tube O'!F18</f>
         <v>1.6845224130000034</v>
       </c>
-      <c r="AT20" s="74">
+      <c r="AQ20" s="74">
         <v>0.22400336766297504</v>
       </c>
-      <c r="AU20" s="72" t="str">
+      <c r="AR20" s="72" t="str">
         <f>'Tube P'!G18</f>
         <v>C11</v>
       </c>
-      <c r="AV20" s="73">
+      <c r="AS20" s="73">
         <f>'Tube P'!F18</f>
         <v>1.6838121190000024</v>
       </c>
-      <c r="AW20" s="74">
+      <c r="AT20" s="74">
         <v>6.9083539541125519E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:49">
+    <row r="21" spans="1:46">
       <c r="A21" s="56">
         <v>18</v>
       </c>
@@ -24878,84 +24504,73 @@
         <v>7.6676197696020285E-2</v>
       </c>
       <c r="AC21" s="72" t="str">
-        <f>'Tube J'!G19</f>
-        <v>H5</v>
-      </c>
-      <c r="AD21" s="70">
-        <f>'Tube J'!F19</f>
-        <v>1.6762447560000009</v>
-      </c>
-      <c r="AE21" s="74">
-        <v>0.13107286315389047</v>
-      </c>
-      <c r="AF21" s="72" t="str">
         <f>'Tube K'!G19</f>
         <v>C8</v>
       </c>
-      <c r="AG21" s="73">
+      <c r="AD21" s="73">
         <f>'Tube K'!F19</f>
         <v>1.6750154010000013</v>
       </c>
-      <c r="AH21" s="74">
+      <c r="AE21" s="74">
         <v>8.280904794884153E-2</v>
       </c>
-      <c r="AI21" s="72" t="str">
+      <c r="AF21" s="72" t="str">
         <f>'Tube L'!G19</f>
         <v>D11</v>
       </c>
-      <c r="AJ21" s="73">
+      <c r="AG21" s="73">
         <f>'Tube L'!F19</f>
         <v>1.6757803330000005</v>
       </c>
-      <c r="AK21" s="74">
+      <c r="AH21" s="74">
         <v>0.19838681034476044</v>
       </c>
-      <c r="AL21" s="72" t="str">
+      <c r="AI21" s="72" t="str">
         <f>'Tube M'!G19</f>
         <v>B3</v>
       </c>
-      <c r="AM21" s="73">
+      <c r="AJ21" s="73">
         <f>'Tube M'!F19</f>
         <v>1.6762993940000008</v>
       </c>
-      <c r="AN21" s="74">
+      <c r="AK21" s="74">
         <v>0.19376664647378908</v>
       </c>
-      <c r="AO21" s="72" t="str">
+      <c r="AL21" s="72" t="str">
         <f>'Tube N'!G19</f>
         <v>H5</v>
       </c>
-      <c r="AP21" s="73">
+      <c r="AM21" s="73">
         <f>'Tube N'!F19</f>
         <v>1.6764906270000015</v>
       </c>
-      <c r="AQ21" s="74">
+      <c r="AN21" s="74">
         <v>0.2071589663723894</v>
       </c>
-      <c r="AR21" s="72" t="str">
+      <c r="AO21" s="72" t="str">
         <f>'Tube O'!G19</f>
         <v>C8</v>
       </c>
-      <c r="AS21" s="73">
+      <c r="AP21" s="73">
         <f>'Tube O'!F19</f>
         <v>1.6757803330000005</v>
       </c>
-      <c r="AT21" s="74">
+      <c r="AQ21" s="74">
         <v>8.2816315557937906E-2</v>
       </c>
-      <c r="AU21" s="72" t="str">
+      <c r="AR21" s="72" t="str">
         <f>'Tube P'!G19</f>
         <v>D11</v>
       </c>
-      <c r="AV21" s="73">
+      <c r="AS21" s="73">
         <f>'Tube P'!F19</f>
         <v>1.6783483190000013</v>
       </c>
-      <c r="AW21" s="74">
+      <c r="AT21" s="74">
         <v>3.0341867447447879E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:49">
+    <row r="22" spans="1:46">
       <c r="A22" s="56">
         <v>19</v>
       </c>
@@ -25059,84 +24674,73 @@
         <v>7.8027755352629832E-2</v>
       </c>
       <c r="AC22" s="72" t="str">
-        <f>'Tube J'!G20</f>
-        <v>H6</v>
-      </c>
-      <c r="AD22" s="70">
-        <f>'Tube J'!F20</f>
-        <v>1.6620388760000022</v>
-      </c>
-      <c r="AE22" s="74">
-        <v>0.1273326074937754</v>
-      </c>
-      <c r="AF22" s="72" t="str">
         <f>'Tube K'!G20</f>
         <v>B8</v>
       </c>
-      <c r="AG22" s="73">
+      <c r="AD22" s="73">
         <f>'Tube K'!F20</f>
         <v>1.6586240010000033</v>
       </c>
-      <c r="AH22" s="74">
+      <c r="AE22" s="74">
         <v>0.10797909932466521</v>
       </c>
-      <c r="AI22" s="72" t="str">
+      <c r="AF22" s="72" t="str">
         <f>'Tube L'!G20</f>
         <v>E11</v>
       </c>
-      <c r="AJ22" s="73">
+      <c r="AG22" s="73">
         <f>'Tube L'!F20</f>
         <v>1.6593889330000025</v>
       </c>
-      <c r="AK22" s="74">
+      <c r="AH22" s="74">
         <v>0.21709354880810086</v>
       </c>
-      <c r="AL22" s="72" t="str">
+      <c r="AI22" s="72" t="str">
         <f>'Tube M'!G20</f>
         <v>C3</v>
       </c>
-      <c r="AM22" s="73">
+      <c r="AJ22" s="73">
         <f>'Tube M'!F20</f>
         <v>1.656629714000001</v>
       </c>
-      <c r="AN22" s="74">
+      <c r="AK22" s="74">
         <v>0.21364413913128055</v>
       </c>
-      <c r="AO22" s="72" t="str">
+      <c r="AL22" s="72" t="str">
         <f>'Tube N'!G20</f>
         <v>H6</v>
       </c>
-      <c r="AP22" s="73">
+      <c r="AM22" s="73">
         <f>'Tube N'!F20</f>
         <v>1.6590064670000029</v>
       </c>
-      <c r="AQ22" s="74">
+      <c r="AN22" s="74">
         <v>0.25119262087491218</v>
       </c>
-      <c r="AR22" s="72" t="str">
+      <c r="AO22" s="72" t="str">
         <f>'Tube O'!G20</f>
         <v>B8</v>
       </c>
-      <c r="AS22" s="73">
+      <c r="AP22" s="73">
         <f>'Tube O'!F20</f>
         <v>1.6495540930000008</v>
       </c>
-      <c r="AT22" s="74">
+      <c r="AQ22" s="74">
         <v>3.8338750332408959E-2</v>
       </c>
-      <c r="AU22" s="72" t="str">
+      <c r="AR22" s="72" t="str">
         <f>'Tube P'!G20</f>
         <v>E11</v>
       </c>
-      <c r="AV22" s="73">
+      <c r="AS22" s="73">
         <f>'Tube P'!F20</f>
         <v>1.663049679000002</v>
       </c>
-      <c r="AW22" s="74">
+      <c r="AT22" s="74">
         <v>1.9575035853108907E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" spans="1:46">
       <c r="A23" s="56">
         <v>20</v>
       </c>
@@ -25240,84 +24844,73 @@
         <v>7.5171430587926844E-2</v>
       </c>
       <c r="AC23" s="72" t="str">
-        <f>'Tube J'!G21</f>
-        <v>G6</v>
-      </c>
-      <c r="AD23" s="70">
-        <f>'Tube J'!F21</f>
-        <v>1.5997515560000011</v>
-      </c>
-      <c r="AE23" s="74">
-        <v>0.16686307307424886</v>
-      </c>
-      <c r="AF23" s="72" t="str">
         <f>'Tube K'!G21</f>
         <v>A8</v>
       </c>
-      <c r="AG23" s="73">
+      <c r="AD23" s="73">
         <f>'Tube K'!F21</f>
         <v>1.603084474000001</v>
       </c>
-      <c r="AH23" s="74">
+      <c r="AE23" s="74">
         <v>0.14106947288055902</v>
       </c>
-      <c r="AI23" s="72" t="str">
+      <c r="AF23" s="72" t="str">
         <f>'Tube L'!G21</f>
         <v>F11</v>
       </c>
-      <c r="AJ23" s="73">
+      <c r="AG23" s="73">
         <f>'Tube L'!F21</f>
         <v>1.5883595330000002</v>
       </c>
-      <c r="AK23" s="74">
+      <c r="AH23" s="74">
         <v>0.20869422311961147</v>
       </c>
-      <c r="AL23" s="72" t="str">
+      <c r="AI23" s="72" t="str">
         <f>'Tube M'!G21</f>
         <v>D3</v>
       </c>
-      <c r="AM23" s="73">
+      <c r="AJ23" s="73">
         <f>'Tube M'!F21</f>
         <v>1.5790437540000024</v>
       </c>
-      <c r="AN23" s="74">
+      <c r="AK23" s="74">
         <v>0.17305113611734502</v>
       </c>
-      <c r="AO23" s="72" t="str">
+      <c r="AL23" s="72" t="str">
         <f>'Tube N'!G21</f>
         <v>G6</v>
       </c>
-      <c r="AP23" s="73">
+      <c r="AM23" s="73">
         <f>'Tube N'!F21</f>
         <v>1.5792349870000013</v>
       </c>
-      <c r="AQ23" s="74">
+      <c r="AN23" s="74">
         <v>0.17991752412575115</v>
       </c>
-      <c r="AR23" s="72" t="str">
+      <c r="AO23" s="72" t="str">
         <f>'Tube O'!G21</f>
         <v>A8</v>
       </c>
-      <c r="AS23" s="73">
+      <c r="AP23" s="73">
         <f>'Tube O'!F21</f>
         <v>1.5621332930000023</v>
       </c>
-      <c r="AT23" s="74">
+      <c r="AQ23" s="74">
         <v>8.0109992244104533E-3</v>
       </c>
-      <c r="AU23" s="72" t="str">
+      <c r="AR23" s="72" t="str">
         <f>'Tube P'!G21</f>
         <v>F11</v>
       </c>
-      <c r="AV23" s="73">
+      <c r="AS23" s="73">
         <f>'Tube P'!F21</f>
         <v>1.5963913190000021</v>
       </c>
-      <c r="AW23" s="74">
+      <c r="AT23" s="74">
         <v>3.8403536199377648E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:49">
+    <row r="24" spans="1:46">
       <c r="A24" s="56">
         <v>21</v>
       </c>
@@ -25421,84 +25014,73 @@
         <v>4.0587666671161399E-2</v>
       </c>
       <c r="AC24" s="69" t="str">
-        <f>'Tube J'!G22</f>
-        <v>F6</v>
-      </c>
-      <c r="AD24" s="70">
-        <f>'Tube J'!F22</f>
-        <v>1.4434868760000015</v>
-      </c>
-      <c r="AE24" s="71">
-        <v>0.11000444170398697</v>
-      </c>
-      <c r="AF24" s="69" t="str">
         <f>'Tube K'!G22</f>
         <v>A9</v>
       </c>
-      <c r="AG24" s="70">
+      <c r="AD24" s="70">
         <f>'Tube K'!F22</f>
         <v>1.4546603470000008</v>
       </c>
-      <c r="AH24" s="71">
+      <c r="AE24" s="71">
         <v>9.2640226623638147E-2</v>
       </c>
-      <c r="AI24" s="69" t="str">
+      <c r="AF24" s="69" t="str">
         <f>'Tube L'!G22</f>
         <v>G11</v>
       </c>
-      <c r="AJ24" s="70">
+      <c r="AG24" s="70">
         <f>'Tube L'!F22</f>
         <v>1.4211672530000019</v>
       </c>
-      <c r="AK24" s="71">
+      <c r="AH24" s="71">
         <v>0.13286403927642432</v>
       </c>
-      <c r="AL24" s="69" t="str">
+      <c r="AI24" s="69" t="str">
         <f>'Tube M'!G22</f>
         <v>E3</v>
       </c>
-      <c r="AM24" s="70">
+      <c r="AJ24" s="70">
         <f>'Tube M'!F22</f>
         <v>1.3987383540000025</v>
       </c>
-      <c r="AN24" s="71">
+      <c r="AK24" s="71">
         <v>6.4530207564664252E-2</v>
       </c>
-      <c r="AO24" s="69" t="str">
+      <c r="AL24" s="69" t="str">
         <f>'Tube N'!G22</f>
         <v>F6</v>
       </c>
-      <c r="AP24" s="70">
+      <c r="AM24" s="70">
         <f>'Tube N'!F22</f>
         <v>1.4043933870000025</v>
       </c>
-      <c r="AQ24" s="71">
+      <c r="AN24" s="71">
         <v>3.1579886490325192E-2</v>
       </c>
-      <c r="AR24" s="69" t="str">
+      <c r="AO24" s="69" t="str">
         <f>'Tube O'!G22</f>
         <v>A9</v>
       </c>
-      <c r="AS24" s="70">
+      <c r="AP24" s="70">
         <f>'Tube O'!F22</f>
         <v>1.3971265330000033</v>
       </c>
-      <c r="AT24" s="71">
+      <c r="AQ24" s="71">
         <v>1.2623115633281836E-2</v>
       </c>
-      <c r="AU24" s="69" t="str">
+      <c r="AR24" s="69" t="str">
         <f>'Tube P'!G22</f>
         <v>G11</v>
       </c>
-      <c r="AV24" s="70">
+      <c r="AS24" s="70">
         <f>'Tube P'!F22</f>
         <v>1.4257295260000014</v>
       </c>
-      <c r="AW24" s="71">
+      <c r="AT24" s="71">
         <v>1.6092599994199739E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:49" ht="13" thickBot="1">
+    <row r="25" spans="1:46" ht="13" thickBot="1">
       <c r="A25" s="56">
         <v>22</v>
       </c>
@@ -25602,84 +25184,73 @@
         <v>2.3568025587256836E-2</v>
       </c>
       <c r="AC25" s="89" t="str">
-        <f>'Tube J'!G23</f>
-        <v>E6</v>
-      </c>
-      <c r="AD25" s="70">
-        <f>'Tube J'!F23</f>
-        <v>1.2273116290000008</v>
-      </c>
-      <c r="AE25" s="71">
-        <v>5.2144187752624215E-2</v>
-      </c>
-      <c r="AF25" s="89" t="str">
         <f>'Tube K'!G23</f>
         <v>B9</v>
       </c>
-      <c r="AG25" s="90">
+      <c r="AD25" s="90">
         <f>'Tube K'!F23</f>
         <v>1.2428561400000024</v>
       </c>
-      <c r="AH25" s="71">
+      <c r="AE25" s="71">
         <v>5.2999835353218804E-2</v>
       </c>
-      <c r="AI25" s="69" t="str">
+      <c r="AF25" s="69" t="str">
         <f>'Tube L'!G23</f>
         <v>H11</v>
       </c>
-      <c r="AJ25" s="90">
+      <c r="AG25" s="90">
         <f>'Tube L'!F23</f>
         <v>1.1982442130000024</v>
       </c>
-      <c r="AK25" s="71">
+      <c r="AH25" s="71">
         <v>7.1588308459175534E-2</v>
       </c>
-      <c r="AL25" s="69" t="str">
+      <c r="AI25" s="69" t="str">
         <f>'Tube M'!G23</f>
         <v>F3</v>
       </c>
-      <c r="AM25" s="70">
+      <c r="AJ25" s="70">
         <f>'Tube M'!F23</f>
         <v>1.1867429140000016</v>
       </c>
-      <c r="AN25" s="71">
+      <c r="AK25" s="71">
         <v>5.0891101741018185E-2</v>
       </c>
-      <c r="AO25" s="89" t="str">
+      <c r="AL25" s="89" t="str">
         <f>'Tube N'!G23</f>
         <v>E6</v>
       </c>
-      <c r="AP25" s="70">
+      <c r="AM25" s="70">
         <f>'Tube N'!F23</f>
         <v>1.1967689870000022</v>
       </c>
-      <c r="AQ25" s="88">
+      <c r="AN25" s="88">
         <v>4.729420319078121E-2</v>
       </c>
-      <c r="AR25" s="69" t="str">
+      <c r="AO25" s="69" t="str">
         <f>'Tube O'!G23</f>
         <v>B9</v>
       </c>
-      <c r="AS25" s="70">
+      <c r="AP25" s="70">
         <f>'Tube O'!F23</f>
         <v>1.2310270130000021</v>
       </c>
-      <c r="AT25" s="88">
+      <c r="AQ25" s="88">
         <v>4.5590295087846733E-2</v>
       </c>
-      <c r="AU25" s="69" t="str">
+      <c r="AR25" s="69" t="str">
         <f>'Tube P'!G23</f>
         <v>H11</v>
       </c>
-      <c r="AV25" s="70">
+      <c r="AS25" s="70">
         <f>'Tube P'!F23</f>
         <v>1.2084615190000019</v>
       </c>
-      <c r="AW25" s="80">
+      <c r="AT25" s="80">
         <v>8.5036801166457079E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:49" ht="13" thickTop="1">
+    <row r="26" spans="1:46" ht="13" thickTop="1">
       <c r="B26" s="73"/>
       <c r="C26" s="81" t="s">
         <v>187</v>
@@ -25753,63 +25324,55 @@
         <v>50.082614944127556</v>
       </c>
       <c r="AC26" s="73"/>
-      <c r="AD26" s="92" t="s">
+      <c r="AD26" s="81" t="s">
         <v>187</v>
       </c>
       <c r="AE26" s="93">
-        <f>SUM(AE5:AE25)*40/'Tube Loading'!K38*100</f>
-        <v>40.552989377242596</v>
-      </c>
-      <c r="AF26" s="73"/>
+        <f>SUM(AE5:AE25)*40/'Tube Loading'!K39*100</f>
+        <v>53.948770902690413</v>
+      </c>
+      <c r="AF26" s="94"/>
       <c r="AG26" s="81" t="s">
         <v>187</v>
       </c>
       <c r="AH26" s="93">
-        <f>SUM(AH5:AH25)*40/'Tube Loading'!K39*100</f>
-        <v>53.948770902690413</v>
-      </c>
-      <c r="AI26" s="94"/>
-      <c r="AJ26" s="81" t="s">
+        <f>SUM(AH5:AH25)*40/'Tube Loading'!K40*100</f>
+        <v>58.371507777243245</v>
+      </c>
+      <c r="AI26" s="91"/>
+      <c r="AJ26" s="92" t="s">
         <v>187</v>
       </c>
       <c r="AK26" s="93">
-        <f>SUM(AK5:AK25)*40/'Tube Loading'!K40*100</f>
-        <v>58.371507777243245</v>
-      </c>
-      <c r="AL26" s="91"/>
+        <f>SUM(AK5:AK25)*40/'Tube Loading'!K41*100</f>
+        <v>75.763760038666732</v>
+      </c>
+      <c r="AL26" s="73"/>
       <c r="AM26" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="AN26" s="93">
-        <f>SUM(AN5:AN25)*40/'Tube Loading'!K41*100</f>
-        <v>75.763760038666732</v>
-      </c>
-      <c r="AO26" s="73"/>
+      <c r="AN26" s="82">
+        <f>SUM(AN5:AN25)*40/'Tube Loading'!K42*100</f>
+        <v>78.869964770790631</v>
+      </c>
+      <c r="AO26" s="91"/>
       <c r="AP26" s="92" t="s">
         <v>187</v>
       </c>
       <c r="AQ26" s="82">
-        <f>SUM(AQ5:AQ25)*40/'Tube Loading'!K42*100</f>
-        <v>78.869964770790631</v>
-      </c>
-      <c r="AR26" s="91"/>
-      <c r="AS26" s="92" t="s">
+        <f>SUM(AQ5:AQ25)*40/'Tube Loading'!K43*100</f>
+        <v>74.347533564064079</v>
+      </c>
+      <c r="AR26" s="83"/>
+      <c r="AS26" s="81" t="s">
         <v>187</v>
       </c>
       <c r="AT26" s="82">
-        <f>SUM(AT5:AT25)*40/'Tube Loading'!K43*100</f>
-        <v>74.347533564064079</v>
-      </c>
-      <c r="AU26" s="83"/>
-      <c r="AV26" s="81" t="s">
-        <v>187</v>
-      </c>
-      <c r="AW26" s="82">
-        <f>SUM(AW5:AW25)*40/'Tube Loading'!K44*100</f>
+        <f>SUM(AT5:AT25)*40/'Tube Loading'!K44*100</f>
         <v>46.076539466850186</v>
       </c>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" spans="1:46">
       <c r="B27" s="73"/>
       <c r="C27" s="73"/>
       <c r="D27" s="73"/>
@@ -25823,7 +25386,7 @@
       <c r="L27" s="73"/>
       <c r="M27" s="73"/>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" spans="1:46">
       <c r="B28" s="73"/>
       <c r="C28" s="73"/>
       <c r="D28" s="73"/>
@@ -25837,13 +25400,13 @@
       <c r="L28" s="73"/>
       <c r="M28" s="73"/>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" spans="1:46">
       <c r="A29" s="62"/>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" spans="1:46">
       <c r="A30" s="62"/>
     </row>
-    <row r="31" spans="1:49">
+    <row r="31" spans="1:46">
       <c r="A31" s="62"/>
     </row>
     <row r="55" spans="1:13">
@@ -25865,10 +25428,10 @@
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="62"/>
-      <c r="B57" s="111"/>
+      <c r="B57" s="109"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="B58" s="111"/>
+      <c r="B58" s="109"/>
     </row>
     <row r="81" spans="1:13">
       <c r="E81" s="73"/>
@@ -25902,15 +25465,7 @@
       <c r="A85" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="AO2:AQ2"/>
-    <mergeCell ref="AR2:AT2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="AL2:AN2"/>
+  <mergeCells count="15">
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="T2:V2"/>
@@ -25919,6 +25474,13 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="AO2:AQ2"/>
+    <mergeCell ref="AR2:AT2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -26380,7 +25942,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="29"/>
@@ -26777,16 +26339,16 @@
         <v>145</v>
       </c>
       <c r="H28" s="101" t="s">
+        <v>209</v>
+      </c>
+      <c r="I28" s="101" t="s">
         <v>210</v>
       </c>
-      <c r="I28" s="101" t="s">
+      <c r="J28" s="101" t="s">
         <v>211</v>
       </c>
-      <c r="J28" s="101" t="s">
-        <v>212</v>
-      </c>
       <c r="K28" s="100" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="14">
@@ -29597,7 +29159,7 @@
         <v>135</v>
       </c>
       <c r="H9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:13">

</xml_diff>